<commit_message>
Aggiornamento check-list e json.data
Aggiornati i file in oggetto in base alla vostra segnalazione
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111DHARMAHEALTHCAREXX/DHARMA/HEALTHNET/0.1/report-checklist.xlsx
+++ b/GATEWAY/A1#111DHARMAHEALTHCAREXX/DHARMA/HEALTHNET/0.1/report-checklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lavoro\Sviluppo\Health.NET Code\FSE Git\GATEWAY\A1#111DHARMAHEALTHCAREXX\DHARMA\HEALTHNET\0.1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lavoro\Sviluppo\Health.NET Code\FSE Git\it-fse-accreditamento\GATEWAY\A1#111DHARMAHEALTHCAREXX\DHARMA\HEALTHNET\0.1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5E2B3CA-13A4-4857-9F20-AC95FE4766CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3534072C-8C16-4B7D-97C4-950E19BE7030}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="1" r:id="rId1"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1447" uniqueCount="551">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1433" uniqueCount="551">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -2757,24 +2757,9 @@
     <t>Il campo action_id non è corretto</t>
   </si>
   <si>
-    <t>Errore di timeout, il referto non è stato inviato</t>
-  </si>
-  <si>
     <t>Il campo purpose_of_use non è valorizzato</t>
   </si>
   <si>
-    <t>2023-07-29T15:00:30Z</t>
-  </si>
-  <si>
-    <t>4ac09fef69e2ed49</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.74e38717aab01fdd42c450a5777ec7bb527899e96906593270e3a09ee4745862.407047a730^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>ERROR: -1,-1 cvc-complex-type.2.4.a: Invalid content was found starting with element \u0027languageCode\u0027. One of \u0027{\urn:hl7-org:v3\":confidentialityCode}\u0027 is expected."</t>
-  </si>
-  <si>
     <t xml:space="preserve">Il software gestionale gestisce a monte (nella scheda di registrazione anagrafica) il controllo del 'case' maiuscolo del Codice Fiscale </t>
   </si>
   <si>
@@ -2799,9 +2784,6 @@
     <t>l'errore che ritorna dal servizio, viene tradotto in "Verificare il numero dell'impegnativa o l'assegnazione del progressivo interno alla richiesta, in caso di richieste non SSN" - L'errore che ritorna dal servizio è: ERROR: -1,-1 cvc-minLength-valid: Value \u0027\u0027 with length = \u00270\u0027 is not facet-valid with respect to minLength \u00271\u0027 for type \u0027st\u0027.,ERROR: -1,-1 cvc-attribute.3: The value \u0027\u0027 of attribute \u0027extension\u0027 on element \u0027id\u0027 is not valid with respect to its type, \u0027st\u0027.</t>
   </si>
   <si>
-    <t>In caso di errori che impediscono il corretto invio, viene generato un Log specifico che viene inoltrato via email al cliente per ogni errore riscontrato. Incaso di errori 'non parlanti' il messaggio di errore viene tradotto in modo che l'operatore possa provvedere a risolverlo</t>
-  </si>
-  <si>
     <t>La gerarchia di section è organizzata seguendo la codifica dei singoli esami nella section foglia (scelta tra le due opzioni proposte nelle specifiche HL7). Pertanto non viene trasmesso nel CDA il dato riguardante la specialità e il test non è applicabile</t>
   </si>
   <si>
@@ -2818,6 +2800,24 @@
   </si>
   <si>
     <t>Il software non prevede la gestione di flussi di laboratorio di centri trasfusionali</t>
+  </si>
+  <si>
+    <t>Il campo purpose_of_use è sempre valorizzato da programma, abbiamo forzatamente rimosso il dato per generare il caso di test KO e per verificare che venisse generato il messaggio di errore leggibile dall'operatore. L'eventuale (improbabile) gestione di questo messaggio da parte dell'operatore, comporta l'apertura di una chiamata al servizio di assistenza per segnalare l'anomalia, in quanto l'operatore non può intervenire direttamente su questo caso di specie.</t>
+  </si>
+  <si>
+    <t>Il campo actionId è sempre valorizzato da programma in modo corretto a seconda del caso corrente; abbiamo forzatamente alterato il dato per generare il caso di test KO e per verificare che venisse generato il messaggio di errore leggibile dall'operatore. L'eventuale (improbabile) gestione di questo messaggio da parte dell'operatore, comporta l'apertura di una chiamata al servizio di assistenza per segnalare l'anomalia, in quanto l'operatore non può intervenire direttamente su questo caso di specie.</t>
+  </si>
+  <si>
+    <t>Errore di timeout, il referto non è stato inviato. Verranno effettuati nuovi tentativi ad intervalli di tempo regolari finchè il servizio non sarà ripristinato</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Non necessita di intervento da parte dell'operatore in quanto il referto rimane in coda di invio finché lo stesso non è andato a buon fine </t>
+  </si>
+  <si>
+    <t>Il campo confidentialityCode è obbligatorio ai fini della produzione del referto, quindi il medico viene avvisato in fase di chiusura del referto e obbligato ad inserire un dato coerente.</t>
+  </si>
+  <si>
+    <t>In caso di errori che impediscono il corretto invio, viene generato un Log specifico che viene inoltrato via email al cliente per ogni errore riscontrato. Incaso di errori 'non parlanti' il messaggio di errore viene tradotto in modo che l'operatore possa provvedere a risolverlo, in questo caso invitandolo esplicitamente a valorizzare il campo richiesto riaprendo la scheda di accettazione del paziente in questione</t>
   </si>
 </sst>
 </file>
@@ -3742,10 +3742,10 @@
   <dimension ref="A1:T1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="G198" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="A384" sqref="A384"/>
+      <selection pane="bottomRight" activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="14.4"/>
@@ -4030,9 +4030,7 @@
         <v>69</v>
       </c>
       <c r="K10" s="25"/>
-      <c r="L10" s="25" t="s">
-        <v>501</v>
-      </c>
+      <c r="L10" s="25"/>
       <c r="M10" s="25"/>
       <c r="N10" s="25"/>
       <c r="O10" s="25"/>
@@ -4078,9 +4076,7 @@
         <v>69</v>
       </c>
       <c r="K11" s="25"/>
-      <c r="L11" s="25" t="s">
-        <v>501</v>
-      </c>
+      <c r="L11" s="25"/>
       <c r="M11" s="25"/>
       <c r="N11" s="25"/>
       <c r="O11" s="25"/>
@@ -4126,9 +4122,7 @@
         <v>69</v>
       </c>
       <c r="K12" s="25"/>
-      <c r="L12" s="25" t="s">
-        <v>501</v>
-      </c>
+      <c r="L12" s="25"/>
       <c r="M12" s="25"/>
       <c r="N12" s="25"/>
       <c r="O12" s="25"/>
@@ -4174,9 +4168,7 @@
         <v>69</v>
       </c>
       <c r="K13" s="25"/>
-      <c r="L13" s="25" t="s">
-        <v>501</v>
-      </c>
+      <c r="L13" s="25"/>
       <c r="M13" s="25"/>
       <c r="N13" s="25"/>
       <c r="O13" s="25"/>
@@ -4222,17 +4214,11 @@
         <v>69</v>
       </c>
       <c r="K14" s="25"/>
-      <c r="L14" s="25" t="s">
-        <v>501</v>
-      </c>
+      <c r="L14" s="25"/>
       <c r="M14" s="25"/>
       <c r="N14" s="25"/>
-      <c r="O14" s="25" t="s">
-        <v>69</v>
-      </c>
-      <c r="P14" s="25" t="s">
-        <v>544</v>
-      </c>
+      <c r="O14" s="25"/>
+      <c r="P14" s="25"/>
       <c r="Q14" s="25" t="s">
         <v>499</v>
       </c>
@@ -4721,13 +4707,13 @@
         <v>69</v>
       </c>
       <c r="N35" s="25" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="O35" s="25" t="s">
-        <v>69</v>
+        <v>501</v>
       </c>
       <c r="P35" s="25" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="Q35" s="25" t="s">
         <v>499</v>
@@ -4934,10 +4920,10 @@
         <v>529</v>
       </c>
       <c r="O43" s="25" t="s">
-        <v>69</v>
+        <v>501</v>
       </c>
       <c r="P43" s="25" t="s">
-        <v>544</v>
+        <v>546</v>
       </c>
       <c r="Q43" s="25" t="s">
         <v>499</v>
@@ -5102,7 +5088,7 @@
       <c r="S50" s="27"/>
       <c r="T50" s="28"/>
     </row>
-    <row r="51" spans="1:20" ht="55.2" customHeight="1">
+    <row r="51" spans="1:20" ht="55.2" customHeight="1" thickBot="1">
       <c r="A51" s="20">
         <v>44</v>
       </c>
@@ -5133,11 +5119,13 @@
         <v>69</v>
       </c>
       <c r="N51" s="25" t="s">
-        <v>530</v>
-      </c>
-      <c r="O51" s="25"/>
+        <v>547</v>
+      </c>
+      <c r="O51" s="25" t="s">
+        <v>501</v>
+      </c>
       <c r="P51" s="25" t="s">
-        <v>544</v>
+        <v>548</v>
       </c>
       <c r="Q51" s="25" t="s">
         <v>499</v>
@@ -5302,7 +5290,7 @@
       <c r="S58" s="27"/>
       <c r="T58" s="28"/>
     </row>
-    <row r="59" spans="1:20" ht="55.2" customHeight="1">
+    <row r="59" spans="1:20" ht="55.2" customHeight="1" thickBot="1">
       <c r="A59" s="20">
         <v>52</v>
       </c>
@@ -5318,47 +5306,29 @@
       <c r="E59" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="F59" s="23">
-        <v>45136</v>
-      </c>
-      <c r="G59" s="24" t="s">
-        <v>532</v>
-      </c>
-      <c r="H59" s="24" t="s">
-        <v>533</v>
-      </c>
-      <c r="I59" s="24" t="s">
-        <v>534</v>
-      </c>
+      <c r="F59" s="23"/>
+      <c r="G59" s="24"/>
+      <c r="H59" s="24"/>
+      <c r="I59" s="24"/>
       <c r="J59" s="25" t="s">
-        <v>69</v>
-      </c>
-      <c r="K59" s="25"/>
-      <c r="L59" s="25" t="s">
         <v>501</v>
       </c>
-      <c r="M59" s="25" t="s">
-        <v>69</v>
-      </c>
-      <c r="N59" s="25" t="s">
-        <v>535</v>
-      </c>
-      <c r="O59" s="25" t="s">
-        <v>69</v>
-      </c>
-      <c r="P59" s="25" t="s">
-        <v>544</v>
-      </c>
-      <c r="Q59" s="25" t="s">
-        <v>499</v>
-      </c>
+      <c r="K59" s="25" t="s">
+        <v>549</v>
+      </c>
+      <c r="L59" s="25"/>
+      <c r="M59" s="25"/>
+      <c r="N59" s="25"/>
+      <c r="O59" s="25"/>
+      <c r="P59" s="25"/>
+      <c r="Q59" s="25"/>
       <c r="R59" s="26"/>
       <c r="S59" s="27"/>
       <c r="T59" s="28" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="60" spans="1:20" ht="55.2" customHeight="1">
+    <row r="60" spans="1:20" ht="55.2" customHeight="1" thickBot="1">
       <c r="A60" s="20">
         <v>53</v>
       </c>
@@ -5382,7 +5352,7 @@
         <v>501</v>
       </c>
       <c r="K60" s="25" t="s">
-        <v>536</v>
+        <v>531</v>
       </c>
       <c r="L60" s="25"/>
       <c r="M60" s="25"/>
@@ -5420,7 +5390,7 @@
         <v>501</v>
       </c>
       <c r="K61" s="25" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="L61" s="25"/>
       <c r="M61" s="25"/>
@@ -5458,7 +5428,7 @@
         <v>501</v>
       </c>
       <c r="K62" s="25" t="s">
-        <v>538</v>
+        <v>533</v>
       </c>
       <c r="L62" s="25"/>
       <c r="M62" s="25"/>
@@ -5496,7 +5466,7 @@
         <v>501</v>
       </c>
       <c r="K63" s="25" t="s">
-        <v>538</v>
+        <v>533</v>
       </c>
       <c r="L63" s="25"/>
       <c r="M63" s="25"/>
@@ -5534,7 +5504,7 @@
         <v>501</v>
       </c>
       <c r="K64" s="25" t="s">
-        <v>538</v>
+        <v>533</v>
       </c>
       <c r="L64" s="25"/>
       <c r="M64" s="25"/>
@@ -5572,7 +5542,7 @@
         <v>501</v>
       </c>
       <c r="K65" s="25" t="s">
-        <v>539</v>
+        <v>534</v>
       </c>
       <c r="L65" s="25"/>
       <c r="M65" s="25"/>
@@ -5606,13 +5576,13 @@
         <v>45136</v>
       </c>
       <c r="G66" s="24" t="s">
-        <v>540</v>
+        <v>535</v>
       </c>
       <c r="H66" s="24" t="s">
-        <v>541</v>
+        <v>536</v>
       </c>
       <c r="I66" s="24" t="s">
-        <v>542</v>
+        <v>537</v>
       </c>
       <c r="J66" s="25" t="s">
         <v>69</v>
@@ -5625,13 +5595,13 @@
         <v>69</v>
       </c>
       <c r="N66" s="25" t="s">
-        <v>543</v>
+        <v>538</v>
       </c>
       <c r="O66" s="25" t="s">
         <v>69</v>
       </c>
       <c r="P66" s="25" t="s">
-        <v>544</v>
+        <v>550</v>
       </c>
       <c r="Q66" s="25" t="s">
         <v>499</v>
@@ -5666,7 +5636,7 @@
         <v>501</v>
       </c>
       <c r="K67" s="25" t="s">
-        <v>545</v>
+        <v>539</v>
       </c>
       <c r="L67" s="25"/>
       <c r="M67" s="25"/>
@@ -5704,7 +5674,7 @@
         <v>501</v>
       </c>
       <c r="K68" s="25" t="s">
-        <v>547</v>
+        <v>541</v>
       </c>
       <c r="L68" s="25"/>
       <c r="M68" s="25"/>
@@ -5742,7 +5712,7 @@
         <v>501</v>
       </c>
       <c r="K69" s="25" t="s">
-        <v>546</v>
+        <v>540</v>
       </c>
       <c r="L69" s="25"/>
       <c r="M69" s="25"/>
@@ -8596,7 +8566,7 @@
         <v>501</v>
       </c>
       <c r="K198" s="25" t="s">
-        <v>550</v>
+        <v>544</v>
       </c>
       <c r="L198" s="25"/>
       <c r="M198" s="25"/>
@@ -14922,10 +14892,10 @@
         <v>45137</v>
       </c>
       <c r="G375" s="24" t="s">
-        <v>548</v>
+        <v>542</v>
       </c>
       <c r="H375" s="24" t="s">
-        <v>549</v>
+        <v>543</v>
       </c>
       <c r="I375" s="24" t="s">
         <v>508</v>
@@ -15126,7 +15096,7 @@
         <v>501</v>
       </c>
       <c r="K383" s="25" t="s">
-        <v>550</v>
+        <v>544</v>
       </c>
       <c r="L383" s="25"/>
       <c r="M383" s="25"/>

</xml_diff>

<commit_message>
Eliminati i casi di test non applicabili a seguito di modifiche necessarie dopo vostra segnalazione. Nuova sottomissione con casi di test ripetuti ex novo e file data.json e report-checklist.xlsx aggiornati di conseguenza
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111DHARMAHEALTHCAREXX/DHARMA/HEALTHNET/0.1/report-checklist.xlsx
+++ b/GATEWAY/A1#111DHARMAHEALTHCAREXX/DHARMA/HEALTHNET/0.1/report-checklist.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lavoro\Sviluppo\Health.NET Code\FSE Git\GATEWAY\A1#111DHARMAHEALTHCAREXX\DHARMA\HEALTHNET\0.1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lavoro\Sviluppo\Health.NET Code\FSE Git\it-fse-accreditamento\GATEWAY\A1#111DHARMAHEALTHCAREXX\DHARMA\HEALTHNET\0.1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5E2B3CA-13A4-4857-9F20-AC95FE4766CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B29013DA-24D8-44AF-A395-EFB5D0652FE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1447" uniqueCount="551">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1417" uniqueCount="543">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -2691,117 +2691,15 @@
     </r>
   </si>
   <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.b46899712bb46fa01bc09e66f7c01366328d6bab1903789d30116e0092170f0f.85140b12d2^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-07-28T15:44:59Z</t>
-  </si>
-  <si>
-    <t>9dcbf0a219ebebb3</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.74e38717aab01fdd42c450a5777ec7bb527899e96906593270e3a09ee4745862.211180f67e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-07-28T15:49:28Z</t>
-  </si>
-  <si>
-    <t>5098c69adfc16c58</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.74e38717aab01fdd42c450a5777ec7bb527899e96906593270e3a09ee4745862.072dd3f925^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-07-28T16:50:16Z</t>
-  </si>
-  <si>
-    <t>23be79c5412c16cb</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.74e38717aab01fdd42c450a5777ec7bb527899e96906593270e3a09ee4745862.85d757d92d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId"</t>
-  </si>
-  <si>
-    <t>2023-07-29T12:54:53Z</t>
-  </si>
-  <si>
-    <t>cdb02976da692700</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.74e38717aab01fdd42c450a5777ec7bb527899e96906593270e3a09ee4745862.575e9abce7^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-07-29T14:07:59Z</t>
-  </si>
-  <si>
-    <t>91493051f4834a63</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.74e38717aab01fdd42c450a5777ec7bb527899e96906593270e3a09ee4745862.a3eecb9ca9^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-07-29T14:25:20Z</t>
-  </si>
-  <si>
-    <t>2751cc4ce542416e</t>
-  </si>
-  <si>
-    <t>UNKNOWN_WORKFLOW_ID</t>
-  </si>
-  <si>
-    <t>2023-07-29T14:48:59Z</t>
-  </si>
-  <si>
-    <t>042a5e752fe9354f</t>
-  </si>
-  <si>
-    <t>Il campo action_id non è corretto</t>
-  </si>
-  <si>
-    <t>Errore di timeout, il referto non è stato inviato</t>
-  </si>
-  <si>
-    <t>Il campo purpose_of_use non è valorizzato</t>
-  </si>
-  <si>
-    <t>2023-07-29T15:00:30Z</t>
-  </si>
-  <si>
-    <t>4ac09fef69e2ed49</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.74e38717aab01fdd42c450a5777ec7bb527899e96906593270e3a09ee4745862.407047a730^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>ERROR: -1,-1 cvc-complex-type.2.4.a: Invalid content was found starting with element \u0027languageCode\u0027. One of \u0027{\urn:hl7-org:v3\":confidentialityCode}\u0027 is expected."</t>
-  </si>
-  <si>
     <t xml:space="preserve">Il software gestionale gestisce a monte (nella scheda di registrazione anagrafica) il controllo del 'case' maiuscolo del Codice Fiscale </t>
   </si>
   <si>
-    <t>di confidenzialità degli esami contenuti nel referto</t>
-  </si>
-  <si>
     <t>Il software effettua una verifica sui dati anagrafici obbligatori prima di procedere all'invio del CDA. In caso di informazioni mancanti avvisa l'utente tramite messaggio a video ed inibisce l'invio.</t>
   </si>
   <si>
     <t>Le uniche due modalità di gestione campioni prevedono lo stato 'Normale' e 'Urgente', correttamente codificate per il CDA. In questo modo non è possibile passare al CDA informazioni scorrette circa questo dato.</t>
   </si>
   <si>
-    <t>2023-07-29T16:32:42Z</t>
-  </si>
-  <si>
-    <t>638ad7c369bb7aa7</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.74e38717aab01fdd42c450a5777ec7bb527899e96906593270e3a09ee4745862.b492d9c2aa^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>l'errore che ritorna dal servizio, viene tradotto in "Verificare il numero dell'impegnativa o l'assegnazione del progressivo interno alla richiesta, in caso di richieste non SSN" - L'errore che ritorna dal servizio è: ERROR: -1,-1 cvc-minLength-valid: Value \u0027\u0027 with length = \u00270\u0027 is not facet-valid with respect to minLength \u00271\u0027 for type \u0027st\u0027.,ERROR: -1,-1 cvc-attribute.3: The value \u0027\u0027 of attribute \u0027extension\u0027 on element \u0027id\u0027 is not valid with respect to its type, \u0027st\u0027.</t>
-  </si>
-  <si>
-    <t>In caso di errori che impediscono il corretto invio, viene generato un Log specifico che viene inoltrato via email al cliente per ogni errore riscontrato. Incaso di errori 'non parlanti' il messaggio di errore viene tradotto in modo che l'operatore possa provvedere a risolverlo</t>
-  </si>
-  <si>
     <t>La gerarchia di section è organizzata seguendo la codifica dei singoli esami nella section foglia (scelta tra le due opzioni proposte nelle specifiche HL7). Pertanto non viene trasmesso nel CDA il dato riguardante la specialità e il test non è applicabile</t>
   </si>
   <si>
@@ -2811,13 +2709,91 @@
     <t>Il software esegue dei controlli formali prima di considerare un referto idoneo all'invio. Tra questi, la presenza del TIPO CAMPIONE su cui è  stato effettuato il test è un dato obbligatorio, senza il quale non si può procedere all'invio del CDA.</t>
   </si>
   <si>
-    <t>2023-07-30T14:13:15Z</t>
-  </si>
-  <si>
-    <t>24af96735c2b5187</t>
-  </si>
-  <si>
     <t>Il software non prevede la gestione di flussi di laboratorio di centri trasfusionali</t>
+  </si>
+  <si>
+    <t>2023-08-06T13:39:34Z</t>
+  </si>
+  <si>
+    <t>4de85c3878ac2d3c</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.74e38717aab01fdd42c450a5777ec7bb527899e96906593270e3a09ee4745862.e51de4d952^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-08-06T13:44:45Z</t>
+  </si>
+  <si>
+    <t>58f6c0ac5048ffb6</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.74e38717aab01fdd42c450a5777ec7bb527899e96906593270e3a09ee4745862.7836146304^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-08-06T13:47:07Z</t>
+  </si>
+  <si>
+    <t>0a1fcfde81d1eff0</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.74e38717aab01fdd42c450a5777ec7bb527899e96906593270e3a09ee4745862.082ef07e70^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-08-06T14:02:36Z</t>
+  </si>
+  <si>
+    <t>23560c097d1aca0a</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.74e38717aab01fdd42c450a5777ec7bb527899e96906593270e3a09ee4745862.5a54a31a83^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-08-06T14:05:31Z</t>
+  </si>
+  <si>
+    <t>b6fc3ed09fc57447</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.74e38717aab01fdd42c450a5777ec7bb527899e96906593270e3a09ee4745862.fd8099bd7b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>Il software richiede l'obbligatorietà dei campi necessari alla generazione dei JWT, in mancanza dei quali non consente la pubblicazione del referto</t>
+  </si>
+  <si>
+    <t>Il software verifica la correttezza dei campi necessari alla generazione dei JWT. In caso di dati non congruenti non consente la pubblicazione del referto.</t>
+  </si>
+  <si>
+    <t>In caso di timeout l'utente riceve un messaggio che lo avvisa del mancato invio del referto al servizio 'Referto non pubblicato: Timeout del servizio di Pubblicazione. Il sistema ripeterà la procedura di invio finché la stessa non andrà a buon fine'. Non si richiede alcuna azione da parte dell'utente in quanto il referto rimane in coda e il software tenta un successivo invio a cadenza temporale di 5 minuti finché l'operazione non va a buon fine.</t>
+  </si>
+  <si>
+    <t>Il software non consente la generazione del referto in caso di mancanza del confidentialityCode</t>
+  </si>
+  <si>
+    <t>Le uniche 2 codifiche possibili del confidentialityCode sono "Normal" e "Very Restricted"</t>
+  </si>
+  <si>
+    <t>2023-08-06T14:29:37Z</t>
+  </si>
+  <si>
+    <t>165d3b3d38bb0b99</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.74e38717aab01fdd42c450a5777ec7bb527899e96906593270e3a09ee4745862.9297c755ee^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>L'errore che ritorna dal servizio, viene tradotto in "Verificare il numero dell'impegnativa o l'assegnazione del progressivo interno alla richiesta, in caso di richieste non SSN" - L'errore che ritorna dal servizio è: ERROR: -1,-1 cvc-minLength-valid: Value \u0027\u0027 with length = \u00270\u0027 is not facet-valid with respect to minLength \u00271\u0027 for type \u0027st\u0027.,ERROR: -1,-1 cvc-attribute.3: The value \u0027\u0027 of attribute \u0027extension\u0027 on element \u0027id\u0027 is not valid with respect to its type, \u0027st\u0027.</t>
+  </si>
+  <si>
+    <t>L'operatore riceve un messaggio a video che lo invita a verificare la presenza del numero impegnativa in caso di ricette SSN o il numero progressivo assegnato automaticamente dal sistema in caso di richieste non SSN. Dopo tale verifica e l'inserimento del dato, può ripetere l'invio del CDA.</t>
+  </si>
+  <si>
+    <t>2023-08-06T14:38:50Z</t>
+  </si>
+  <si>
+    <t>3b1d761068f3abbe</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.74e38717aab01fdd42c450a5777ec7bb527899e96906593270e3a09ee4745862.d3b30ac140^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -3742,10 +3718,10 @@
   <dimension ref="A1:T1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="G198" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="A384" sqref="A384"/>
+      <selection pane="bottomRight" activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="14.4"/>
@@ -4015,16 +3991,16 @@
         <v>45</v>
       </c>
       <c r="F10" s="23">
-        <v>45135</v>
+        <v>45144</v>
       </c>
       <c r="G10" s="24" t="s">
-        <v>509</v>
+        <v>515</v>
       </c>
       <c r="H10" s="24" t="s">
-        <v>510</v>
+        <v>516</v>
       </c>
       <c r="I10" s="24" t="s">
-        <v>511</v>
+        <v>517</v>
       </c>
       <c r="J10" s="25" t="s">
         <v>69</v>
@@ -4063,16 +4039,16 @@
         <v>48</v>
       </c>
       <c r="F11" s="23">
-        <v>45135</v>
+        <v>45144</v>
       </c>
       <c r="G11" s="24" t="s">
-        <v>512</v>
+        <v>518</v>
       </c>
       <c r="H11" s="24" t="s">
-        <v>513</v>
+        <v>519</v>
       </c>
       <c r="I11" s="24" t="s">
-        <v>514</v>
+        <v>520</v>
       </c>
       <c r="J11" s="25" t="s">
         <v>69</v>
@@ -4111,16 +4087,16 @@
         <v>50</v>
       </c>
       <c r="F12" s="23">
-        <v>45135</v>
+        <v>45144</v>
       </c>
       <c r="G12" s="24" t="s">
-        <v>515</v>
+        <v>521</v>
       </c>
       <c r="H12" s="24" t="s">
-        <v>516</v>
+        <v>522</v>
       </c>
       <c r="I12" s="24" t="s">
-        <v>517</v>
+        <v>523</v>
       </c>
       <c r="J12" s="25" t="s">
         <v>69</v>
@@ -4159,16 +4135,16 @@
         <v>52</v>
       </c>
       <c r="F13" s="23">
-        <v>45136</v>
+        <v>45144</v>
       </c>
       <c r="G13" s="24" t="s">
-        <v>518</v>
+        <v>524</v>
       </c>
       <c r="H13" s="24" t="s">
-        <v>519</v>
+        <v>525</v>
       </c>
       <c r="I13" s="24" t="s">
-        <v>520</v>
+        <v>526</v>
       </c>
       <c r="J13" s="25" t="s">
         <v>69</v>
@@ -4207,16 +4183,16 @@
         <v>54</v>
       </c>
       <c r="F14" s="23">
-        <v>45136</v>
+        <v>45144</v>
       </c>
       <c r="G14" s="24" t="s">
-        <v>521</v>
+        <v>527</v>
       </c>
       <c r="H14" s="24" t="s">
-        <v>522</v>
+        <v>528</v>
       </c>
       <c r="I14" s="24" t="s">
-        <v>523</v>
+        <v>529</v>
       </c>
       <c r="J14" s="25" t="s">
         <v>69</v>
@@ -4227,12 +4203,8 @@
       </c>
       <c r="M14" s="25"/>
       <c r="N14" s="25"/>
-      <c r="O14" s="25" t="s">
-        <v>69</v>
-      </c>
-      <c r="P14" s="25" t="s">
-        <v>544</v>
-      </c>
+      <c r="O14" s="25"/>
+      <c r="P14" s="25"/>
       <c r="Q14" s="25" t="s">
         <v>499</v>
       </c>
@@ -4698,40 +4670,22 @@
       <c r="E35" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="F35" s="23">
-        <v>45136</v>
-      </c>
-      <c r="G35" s="24" t="s">
-        <v>524</v>
-      </c>
-      <c r="H35" s="24" t="s">
-        <v>525</v>
-      </c>
-      <c r="I35" s="24" t="s">
-        <v>526</v>
-      </c>
+      <c r="F35" s="23"/>
+      <c r="G35" s="24"/>
+      <c r="H35" s="24"/>
+      <c r="I35" s="24"/>
       <c r="J35" s="25" t="s">
-        <v>69</v>
-      </c>
-      <c r="K35" s="25"/>
-      <c r="L35" s="25" t="s">
         <v>501</v>
       </c>
-      <c r="M35" s="25" t="s">
-        <v>69</v>
-      </c>
-      <c r="N35" s="25" t="s">
-        <v>531</v>
-      </c>
-      <c r="O35" s="25" t="s">
-        <v>69</v>
-      </c>
-      <c r="P35" s="25" t="s">
-        <v>544</v>
-      </c>
-      <c r="Q35" s="25" t="s">
-        <v>499</v>
-      </c>
+      <c r="K35" s="25" t="s">
+        <v>530</v>
+      </c>
+      <c r="L35" s="25"/>
+      <c r="M35" s="25"/>
+      <c r="N35" s="25"/>
+      <c r="O35" s="25"/>
+      <c r="P35" s="25"/>
+      <c r="Q35" s="25"/>
       <c r="R35" s="26"/>
       <c r="S35" s="27"/>
       <c r="T35" s="28" t="s">
@@ -4908,40 +4862,22 @@
       <c r="E43" s="22" t="s">
         <v>66</v>
       </c>
-      <c r="F43" s="23">
-        <v>45136</v>
-      </c>
-      <c r="G43" s="24" t="s">
-        <v>527</v>
-      </c>
-      <c r="H43" s="24" t="s">
-        <v>528</v>
-      </c>
-      <c r="I43" s="24" t="s">
-        <v>526</v>
-      </c>
+      <c r="F43" s="23"/>
+      <c r="G43" s="24"/>
+      <c r="H43" s="24"/>
+      <c r="I43" s="24"/>
       <c r="J43" s="25" t="s">
-        <v>69</v>
-      </c>
-      <c r="K43" s="25"/>
-      <c r="L43" s="25" t="s">
         <v>501</v>
       </c>
-      <c r="M43" s="25" t="s">
-        <v>69</v>
-      </c>
-      <c r="N43" s="25" t="s">
-        <v>529</v>
-      </c>
-      <c r="O43" s="25" t="s">
-        <v>69</v>
-      </c>
-      <c r="P43" s="25" t="s">
-        <v>544</v>
-      </c>
-      <c r="Q43" s="25" t="s">
-        <v>499</v>
-      </c>
+      <c r="K43" s="25" t="s">
+        <v>531</v>
+      </c>
+      <c r="L43" s="25"/>
+      <c r="M43" s="25"/>
+      <c r="N43" s="25"/>
+      <c r="O43" s="25"/>
+      <c r="P43" s="25"/>
+      <c r="Q43" s="25"/>
       <c r="R43" s="26"/>
       <c r="S43" s="27"/>
       <c r="T43" s="28" t="s">
@@ -5126,22 +5062,14 @@
         <v>69</v>
       </c>
       <c r="K51" s="25"/>
-      <c r="L51" s="25" t="s">
-        <v>501</v>
-      </c>
-      <c r="M51" s="25" t="s">
-        <v>69</v>
-      </c>
-      <c r="N51" s="25" t="s">
-        <v>530</v>
-      </c>
+      <c r="L51" s="25"/>
+      <c r="M51" s="25"/>
+      <c r="N51" s="25"/>
       <c r="O51" s="25"/>
       <c r="P51" s="25" t="s">
-        <v>544</v>
-      </c>
-      <c r="Q51" s="25" t="s">
-        <v>499</v>
-      </c>
+        <v>532</v>
+      </c>
+      <c r="Q51" s="25"/>
       <c r="R51" s="26"/>
       <c r="S51" s="27"/>
       <c r="T51" s="28" t="s">
@@ -5318,40 +5246,22 @@
       <c r="E59" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="F59" s="23">
-        <v>45136</v>
-      </c>
-      <c r="G59" s="24" t="s">
-        <v>532</v>
-      </c>
-      <c r="H59" s="24" t="s">
+      <c r="F59" s="23"/>
+      <c r="G59" s="24"/>
+      <c r="H59" s="24"/>
+      <c r="I59" s="24"/>
+      <c r="J59" s="25" t="s">
+        <v>501</v>
+      </c>
+      <c r="K59" s="25" t="s">
         <v>533</v>
       </c>
-      <c r="I59" s="24" t="s">
-        <v>534</v>
-      </c>
-      <c r="J59" s="25" t="s">
-        <v>69</v>
-      </c>
-      <c r="K59" s="25"/>
-      <c r="L59" s="25" t="s">
-        <v>501</v>
-      </c>
-      <c r="M59" s="25" t="s">
-        <v>69</v>
-      </c>
-      <c r="N59" s="25" t="s">
-        <v>535</v>
-      </c>
-      <c r="O59" s="25" t="s">
-        <v>69</v>
-      </c>
-      <c r="P59" s="25" t="s">
-        <v>544</v>
-      </c>
-      <c r="Q59" s="25" t="s">
-        <v>499</v>
-      </c>
+      <c r="L59" s="25"/>
+      <c r="M59" s="25"/>
+      <c r="N59" s="25"/>
+      <c r="O59" s="25"/>
+      <c r="P59" s="25"/>
+      <c r="Q59" s="25"/>
       <c r="R59" s="26"/>
       <c r="S59" s="27"/>
       <c r="T59" s="28" t="s">
@@ -5382,7 +5292,7 @@
         <v>501</v>
       </c>
       <c r="K60" s="25" t="s">
-        <v>536</v>
+        <v>508</v>
       </c>
       <c r="L60" s="25"/>
       <c r="M60" s="25"/>
@@ -5420,7 +5330,7 @@
         <v>501</v>
       </c>
       <c r="K61" s="25" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="L61" s="25"/>
       <c r="M61" s="25"/>
@@ -5458,7 +5368,7 @@
         <v>501</v>
       </c>
       <c r="K62" s="25" t="s">
-        <v>538</v>
+        <v>509</v>
       </c>
       <c r="L62" s="25"/>
       <c r="M62" s="25"/>
@@ -5496,7 +5406,7 @@
         <v>501</v>
       </c>
       <c r="K63" s="25" t="s">
-        <v>538</v>
+        <v>509</v>
       </c>
       <c r="L63" s="25"/>
       <c r="M63" s="25"/>
@@ -5534,7 +5444,7 @@
         <v>501</v>
       </c>
       <c r="K64" s="25" t="s">
-        <v>538</v>
+        <v>509</v>
       </c>
       <c r="L64" s="25"/>
       <c r="M64" s="25"/>
@@ -5572,7 +5482,7 @@
         <v>501</v>
       </c>
       <c r="K65" s="25" t="s">
-        <v>539</v>
+        <v>510</v>
       </c>
       <c r="L65" s="25"/>
       <c r="M65" s="25"/>
@@ -5603,16 +5513,16 @@
         <v>85</v>
       </c>
       <c r="F66" s="23">
-        <v>45136</v>
+        <v>45144</v>
       </c>
       <c r="G66" s="24" t="s">
-        <v>540</v>
+        <v>535</v>
       </c>
       <c r="H66" s="24" t="s">
-        <v>541</v>
+        <v>536</v>
       </c>
       <c r="I66" s="24" t="s">
-        <v>542</v>
+        <v>537</v>
       </c>
       <c r="J66" s="25" t="s">
         <v>69</v>
@@ -5625,13 +5535,13 @@
         <v>69</v>
       </c>
       <c r="N66" s="25" t="s">
-        <v>543</v>
+        <v>538</v>
       </c>
       <c r="O66" s="25" t="s">
         <v>69</v>
       </c>
       <c r="P66" s="25" t="s">
-        <v>544</v>
+        <v>539</v>
       </c>
       <c r="Q66" s="25" t="s">
         <v>499</v>
@@ -5666,7 +5576,7 @@
         <v>501</v>
       </c>
       <c r="K67" s="25" t="s">
-        <v>545</v>
+        <v>511</v>
       </c>
       <c r="L67" s="25"/>
       <c r="M67" s="25"/>
@@ -5704,7 +5614,7 @@
         <v>501</v>
       </c>
       <c r="K68" s="25" t="s">
-        <v>547</v>
+        <v>513</v>
       </c>
       <c r="L68" s="25"/>
       <c r="M68" s="25"/>
@@ -5742,7 +5652,7 @@
         <v>501</v>
       </c>
       <c r="K69" s="25" t="s">
-        <v>546</v>
+        <v>512</v>
       </c>
       <c r="L69" s="25"/>
       <c r="M69" s="25"/>
@@ -8596,7 +8506,7 @@
         <v>501</v>
       </c>
       <c r="K198" s="25" t="s">
-        <v>550</v>
+        <v>514</v>
       </c>
       <c r="L198" s="25"/>
       <c r="M198" s="25"/>
@@ -14919,16 +14829,16 @@
         <v>445</v>
       </c>
       <c r="F375" s="23">
-        <v>45137</v>
+        <v>45144</v>
       </c>
       <c r="G375" s="24" t="s">
-        <v>548</v>
+        <v>540</v>
       </c>
       <c r="H375" s="24" t="s">
-        <v>549</v>
+        <v>541</v>
       </c>
       <c r="I375" s="24" t="s">
-        <v>508</v>
+        <v>542</v>
       </c>
       <c r="J375" s="25" t="s">
         <v>69</v>
@@ -15126,7 +15036,7 @@
         <v>501</v>
       </c>
       <c r="K383" s="25" t="s">
-        <v>550</v>
+        <v>514</v>
       </c>
       <c r="L383" s="25"/>
       <c r="M383" s="25"/>

</xml_diff>